<commit_message>
I summed the total costs of what we each spent on the project.
</commit_message>
<xml_diff>
--- a/Bill of Material v.3.xlsx
+++ b/Bill of Material v.3.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Steel Bridge/Users/metalmachine/Speed Demon/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="51120" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="19420" windowHeight="11020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="139">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -435,16 +430,25 @@
   </si>
   <si>
     <t>COST OF SINGLE UNIT</t>
+  </si>
+  <si>
+    <t>Zach spent</t>
+  </si>
+  <si>
+    <t>Nathan spent</t>
+  </si>
+  <si>
+    <t>Andrew spent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -606,13 +610,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,21 +889,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="14.33203125" style="3" customWidth="1"/>
@@ -912,22 +916,22 @@
     <col min="10" max="16384" width="10.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="I1" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -954,7 +958,7 @@
         <v>106.9525</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -977,7 +981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1001,7 +1005,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>62.832000000000015</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1052,7 +1056,7 @@
       </c>
       <c r="I6" s="21"/>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1074,9 +1078,11 @@
       <c r="G7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="22"/>
-    </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1094,8 +1100,12 @@
       <c r="G8" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="24">
+        <f>SUM(D5:D9,D13,D19:D21,D23:D59)</f>
+        <v>274.33999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1116,7 +1126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -1138,8 +1148,11 @@
       <c r="G10" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -1161,8 +1174,12 @@
       <c r="G11" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <f>SUM(D3:D4,D10:D12,D22)</f>
+        <v>78.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1185,7 +1202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -1201,8 +1218,11 @@
         <v>6</v>
       </c>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
@@ -1220,8 +1240,12 @@
       <c r="G14" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <f>SUM(D14:D18)</f>
+        <v>75.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
@@ -1240,7 +1264,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>36</v>
       </c>
@@ -1261,7 +1285,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>38</v>
       </c>
@@ -1280,7 +1304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>39</v>
       </c>
@@ -1299,7 +1323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>44</v>
       </c>
@@ -1320,7 +1344,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -1341,7 +1365,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
@@ -1360,7 +1384,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>57</v>
       </c>
@@ -1383,7 +1407,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A23" s="15" t="s">
         <v>58</v>
       </c>
@@ -1408,7 +1432,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A24" s="15" t="s">
         <v>60</v>
       </c>
@@ -1433,7 +1457,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A25" s="15" t="s">
         <v>62</v>
       </c>
@@ -1458,7 +1482,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A26" s="15" t="s">
         <v>64</v>
       </c>
@@ -1483,7 +1507,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A27" s="15" t="s">
         <v>66</v>
       </c>
@@ -1508,7 +1532,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A28" s="15" t="s">
         <v>68</v>
       </c>
@@ -1533,7 +1557,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A29" s="15" t="s">
         <v>70</v>
       </c>
@@ -1558,7 +1582,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="15" t="s">
         <v>72</v>
       </c>
@@ -1583,7 +1607,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="21">
       <c r="A31" s="15" t="s">
         <v>74</v>
       </c>
@@ -1608,7 +1632,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="21">
       <c r="A32" s="15" t="s">
         <v>76</v>
       </c>
@@ -1633,7 +1657,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="21">
       <c r="A33" s="15" t="s">
         <v>79</v>
       </c>
@@ -1658,7 +1682,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="21">
       <c r="A34" s="15" t="s">
         <v>81</v>
       </c>
@@ -1683,7 +1707,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="21">
       <c r="A35" s="15" t="s">
         <v>83</v>
       </c>
@@ -1708,7 +1732,7 @@
       <c r="H35" s="14"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="21">
       <c r="A36" s="15" t="s">
         <v>85</v>
       </c>
@@ -1733,7 +1757,7 @@
       <c r="H36" s="14"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="21">
       <c r="A37" s="15" t="s">
         <v>87</v>
       </c>
@@ -1758,7 +1782,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="21">
       <c r="A38" s="15" t="s">
         <v>89</v>
       </c>
@@ -1783,7 +1807,7 @@
       <c r="H38" s="14"/>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="21">
       <c r="A39" s="15" t="s">
         <v>91</v>
       </c>
@@ -1808,7 +1832,7 @@
       <c r="H39" s="14"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="21">
       <c r="A40" s="15" t="s">
         <v>93</v>
       </c>
@@ -1833,7 +1857,7 @@
       <c r="H40" s="14"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="21">
       <c r="A41" s="15" t="s">
         <v>95</v>
       </c>
@@ -1858,7 +1882,7 @@
       <c r="H41" s="14"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="21">
       <c r="A42" s="15" t="s">
         <v>97</v>
       </c>
@@ -1883,7 +1907,7 @@
       <c r="H42" s="14"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="21">
       <c r="A43" s="15" t="s">
         <v>99</v>
       </c>
@@ -1908,7 +1932,7 @@
       <c r="H43" s="14"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="21">
       <c r="A44" s="15" t="s">
         <v>101</v>
       </c>
@@ -1933,7 +1957,7 @@
       <c r="H44" s="14"/>
       <c r="I44" s="11"/>
     </row>
-    <row r="45" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="21">
       <c r="A45" s="15" t="s">
         <v>103</v>
       </c>
@@ -1958,7 +1982,7 @@
       <c r="H45" s="14"/>
       <c r="I45" s="11"/>
     </row>
-    <row r="46" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="21">
       <c r="A46" s="15" t="s">
         <v>105</v>
       </c>
@@ -1983,7 +2007,7 @@
       <c r="H46" s="14"/>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="21">
       <c r="A47" s="15" t="s">
         <v>107</v>
       </c>
@@ -2008,7 +2032,7 @@
       <c r="H47" s="14"/>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="21">
       <c r="A48" s="15" t="s">
         <v>109</v>
       </c>
@@ -2033,7 +2057,7 @@
       <c r="H48" s="14"/>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="21">
       <c r="A49" s="15" t="s">
         <v>111</v>
       </c>
@@ -2058,7 +2082,7 @@
       <c r="H49" s="14"/>
       <c r="I49" s="11"/>
     </row>
-    <row r="50" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="21">
       <c r="A50" s="15" t="s">
         <v>113</v>
       </c>
@@ -2083,7 +2107,7 @@
       <c r="H50" s="14"/>
       <c r="I50" s="11"/>
     </row>
-    <row r="51" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="21">
       <c r="A51" s="15" t="s">
         <v>115</v>
       </c>
@@ -2108,7 +2132,7 @@
       <c r="H51" s="14"/>
       <c r="I51" s="11"/>
     </row>
-    <row r="52" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="21">
       <c r="A52" s="15" t="s">
         <v>117</v>
       </c>
@@ -2133,7 +2157,7 @@
       <c r="H52" s="14"/>
       <c r="I52" s="11"/>
     </row>
-    <row r="53" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="21">
       <c r="A53" s="15" t="s">
         <v>119</v>
       </c>
@@ -2158,7 +2182,7 @@
       <c r="H53" s="14"/>
       <c r="I53" s="11"/>
     </row>
-    <row r="54" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="21">
       <c r="A54" s="15" t="s">
         <v>121</v>
       </c>
@@ -2183,7 +2207,7 @@
       <c r="H54" s="14"/>
       <c r="I54" s="11"/>
     </row>
-    <row r="55" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="21">
       <c r="A55" s="15" t="s">
         <v>123</v>
       </c>
@@ -2208,7 +2232,7 @@
       <c r="H55" s="14"/>
       <c r="I55" s="11"/>
     </row>
-    <row r="56" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="21">
       <c r="A56" s="15" t="s">
         <v>125</v>
       </c>
@@ -2233,7 +2257,7 @@
       <c r="H56" s="14"/>
       <c r="I56" s="11"/>
     </row>
-    <row r="57" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="21">
       <c r="A57" s="15" t="s">
         <v>127</v>
       </c>
@@ -2258,7 +2282,7 @@
       <c r="H57" s="14"/>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="21">
       <c r="A58" s="15" t="s">
         <v>129</v>
       </c>
@@ -2283,7 +2307,7 @@
       <c r="H58" s="14"/>
       <c r="I58" s="11"/>
     </row>
-    <row r="59" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="21">
       <c r="A59" s="15" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
I added in the price of one more MCU that Andrew had purchased.
</commit_message>
<xml_diff>
--- a/Bill of Material v.3.xlsx
+++ b/Bill of Material v.3.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="139">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -565,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -610,13 +610,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -917,15 +920,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="I1" s="8" t="s">
         <v>50</v>
       </c>
@@ -955,7 +958,7 @@
       </c>
       <c r="I2" s="9">
         <f>SUM(D3:D96)/4</f>
-        <v>106.9525</v>
+        <v>109.16500000000001</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
@@ -1100,7 +1103,7 @@
       <c r="G8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="22">
         <f>SUM(D5:D9,D13,D19:D21,D23:D59)</f>
         <v>274.33999999999992</v>
       </c>
@@ -1241,8 +1244,8 @@
         <v>43</v>
       </c>
       <c r="I14" s="2">
-        <f>SUM(D14:D18)</f>
-        <v>75.13</v>
+        <f>SUM(D14:D18,D60)</f>
+        <v>83.97999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
@@ -2331,6 +2334,22 @@
       </c>
       <c r="H59" s="14"/>
       <c r="I59" s="11"/>
+    </row>
+    <row r="60" spans="1:9" ht="21">
+      <c r="A60" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" s="25">
+        <v>1</v>
+      </c>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25">
+        <v>8.85</v>
+      </c>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>